<commit_message>
S41 App7 158 Sending a Single Email
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -11,15 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
-    <t>Table 1</t>
+    <t>name</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Surname</t>
+    <t>surname</t>
   </si>
   <si>
     <t>email</t>
@@ -38,14 +35,14 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="8"/>
+        <color indexed="15"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>pythonprocourse2@gmail.com</t>
+      <t>ypddjuio@yomail.info</t>
     </r>
   </si>
   <si>
-    <t>Meditation</t>
+    <t>meditation</t>
   </si>
   <si>
     <t>Marry</t>
@@ -55,14 +52,31 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="8"/>
+        <color indexed="15"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>pythonprocourse3@gmail.com</t>
+      <t>kawnlyiw@supere.ml</t>
     </r>
   </si>
   <si>
-    <t>Nasa</t>
+    <t>nasa</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Kann</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>pythonprocourse2@gmail.com</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -72,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -80,6 +94,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -92,11 +111,11 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="8"/>
+      <color indexed="15"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,8 +134,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -137,6 +162,19 @@
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -189,6 +227,17 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -229,56 +278,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -301,7 +438,10 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -318,10 +458,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -498,11 +638,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -511,33 +654,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -554,6 +698,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -579,6 +724,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -604,6 +750,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -629,6 +776,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -654,6 +802,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -679,6 +828,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -704,6 +854,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -729,6 +880,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -754,6 +906,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -776,12 +929,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -804,6 +957,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -829,6 +983,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -854,6 +1009,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -879,6 +1035,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -904,6 +1061,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -929,6 +1087,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -954,6 +1113,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -979,6 +1139,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1004,6 +1165,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1029,6 +1191,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1062,20 +1225,21 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1105,6 +1269,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1130,6 +1295,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1155,6 +1321,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1180,6 +1347,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1205,6 +1373,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1230,6 +1399,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1255,6 +1425,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1280,6 +1451,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1305,6 +1477,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
+          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1330,108 +1503,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G6"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.35156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.35156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="3">
+      <c r="A2" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" ht="32.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="B2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="C2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="D2" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" ht="32.05" customHeight="1">
-      <c r="A4" t="s" s="9">
+      <c r="B3" t="s" s="9">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="10">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="11">
+      <c r="D3" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" t="s" s="8">
         <v>11</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="B4" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7"/>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="E5" s="13"/>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" location="" tooltip="" display="pythonprocourse2@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId2" location="" tooltip="" display="pythonprocourse3@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="ypddjuio@yomail.info"/>
+    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="kawnlyiw@supere.ml"/>
+    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display="pythonprocourse2@gmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>